<commit_message>
login, search for ver.2
</commit_message>
<xml_diff>
--- a/Test_02.xlsx
+++ b/Test_02.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="438">
   <si>
     <t>結合テスト</t>
     <rPh sb="0" eb="2">
@@ -3668,12 +3668,155 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>18ー1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.phpからregist.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」でログインしているとき、urlでregist.phpと打つ。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.phpからlist.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.phpからdelete.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.phpからupdate.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>18ー2</t>
+  </si>
+  <si>
+    <t>18ー3</t>
+  </si>
+  <si>
+    <t>18ー4</t>
+  </si>
+  <si>
+    <t>「一般」でログインしているとき、urlでlist.phpと打つ。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」でログインしているとき、urlでdelete.phpと打つ。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」でログインしているとき、urlでupdate.phpと打つ。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」であるので、アカウント登録画面の表示はさせない。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」であるので、アカウントi一覧画面の表示はさせない。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」であるので、アカウント削除画面の表示はさせない。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」であるので、アカウント更新画面の表示はさせない。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一般」であるのに遷移してしまう。</t>
+    <rPh sb="1" eb="3">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>センイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4097,13 +4240,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:K169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J156" sqref="J156"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="J169" sqref="J169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="35.33203125" customWidth="1"/>
@@ -4117,13 +4260,13 @@
     <col min="10" max="10" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -4153,7 +4296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4183,7 +4326,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="26.4" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -4213,7 +4356,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="33" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>102</v>
       </c>
@@ -4243,7 +4386,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="33.6" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
@@ -4273,7 +4416,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="26.4">
       <c r="A7" s="3" t="s">
         <v>104</v>
       </c>
@@ -4303,7 +4446,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="26.4">
       <c r="A8" s="3" t="s">
         <v>105</v>
       </c>
@@ -4333,7 +4476,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="26.4">
       <c r="A9" s="3" t="s">
         <v>106</v>
       </c>
@@ -4363,7 +4506,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="52.8">
       <c r="A10" s="3" t="s">
         <v>107</v>
       </c>
@@ -4393,7 +4536,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="26.4">
       <c r="A11" s="3" t="s">
         <v>108</v>
       </c>
@@ -4423,7 +4566,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="26.4">
       <c r="A12" s="3" t="s">
         <v>109</v>
       </c>
@@ -4453,7 +4596,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="26.4">
       <c r="A13" s="3" t="s">
         <v>110</v>
       </c>
@@ -4483,7 +4626,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="26.4">
       <c r="A14" s="3" t="s">
         <v>111</v>
       </c>
@@ -4513,7 +4656,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="26.4">
       <c r="A15" s="3" t="s">
         <v>112</v>
       </c>
@@ -4543,7 +4686,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="26.4">
       <c r="A16" s="3" t="s">
         <v>122</v>
       </c>
@@ -4573,7 +4716,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="26.4">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -4603,7 +4746,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="55.2" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -4633,7 +4776,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="45.6" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -4663,7 +4806,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="39.6">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -4693,7 +4836,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="39.6">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -4723,7 +4866,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="39.6">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -4753,7 +4896,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="39.6">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -4783,7 +4926,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="39.6">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -4813,7 +4956,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="39.6">
       <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
@@ -4843,7 +4986,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="39.6">
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
@@ -4873,7 +5016,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="39.6">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -4903,7 +5046,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="42.6" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
@@ -4933,7 +5076,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="43.2" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
@@ -4963,7 +5106,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="52.8">
       <c r="A30" s="3" t="s">
         <v>55</v>
       </c>
@@ -4993,7 +5136,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="39.6">
       <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
@@ -5023,7 +5166,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="39.6">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -5053,7 +5196,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="39.6">
       <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
@@ -5083,7 +5226,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="39.6">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
@@ -5113,7 +5256,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="39.6">
       <c r="A35" s="3" t="s">
         <v>60</v>
       </c>
@@ -5143,7 +5286,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="79.2">
       <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
@@ -5173,7 +5316,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="52.8">
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
@@ -5203,7 +5346,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="39.6">
       <c r="A38" s="3" t="s">
         <v>66</v>
       </c>
@@ -5233,7 +5376,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="39.6">
       <c r="A39" s="3" t="s">
         <v>67</v>
       </c>
@@ -5263,7 +5406,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="39.6">
       <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
@@ -5293,7 +5436,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="39.6">
       <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
@@ -5323,7 +5466,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="52.8">
       <c r="A42" s="3" t="s">
         <v>83</v>
       </c>
@@ -5353,7 +5496,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="39.6">
       <c r="A43" s="3" t="s">
         <v>100</v>
       </c>
@@ -5383,7 +5526,7 @@
         <v>45404</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="26.4">
       <c r="A44" s="3" t="s">
         <v>100</v>
       </c>
@@ -5413,7 +5556,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="52.8">
       <c r="A46" s="1">
         <v>5</v>
       </c>
@@ -5443,7 +5586,7 @@
         <v>45398</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="24.6" customHeight="1">
       <c r="A47" s="9" t="s">
         <v>126</v>
       </c>
@@ -5473,7 +5616,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="39.6">
       <c r="A48" s="9" t="s">
         <v>157</v>
       </c>
@@ -5503,7 +5646,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="39.6">
       <c r="A49" s="9" t="s">
         <v>158</v>
       </c>
@@ -5533,7 +5676,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="39.6">
       <c r="A50" s="9" t="s">
         <v>159</v>
       </c>
@@ -5563,7 +5706,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="39.6">
       <c r="A51" s="9" t="s">
         <v>160</v>
       </c>
@@ -5593,7 +5736,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="39.6">
       <c r="A52" s="9" t="s">
         <v>161</v>
       </c>
@@ -5623,7 +5766,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="46.8" customHeight="1">
       <c r="A53" s="9" t="s">
         <v>162</v>
       </c>
@@ -5653,7 +5796,7 @@
         <v>45404</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="54.6" customHeight="1">
       <c r="A54" s="9" t="s">
         <v>163</v>
       </c>
@@ -5683,7 +5826,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="54.6" customHeight="1">
       <c r="A55" s="9" t="s">
         <v>164</v>
       </c>
@@ -5713,7 +5856,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="46.8" customHeight="1">
       <c r="A56" s="9" t="s">
         <v>165</v>
       </c>
@@ -5743,7 +5886,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="39.6">
       <c r="A57" s="9" t="s">
         <v>166</v>
       </c>
@@ -5773,7 +5916,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="26.4">
       <c r="A58" s="9" t="s">
         <v>167</v>
       </c>
@@ -5805,7 +5948,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="26.4">
       <c r="A59" s="9" t="s">
         <v>168</v>
       </c>
@@ -5837,7 +5980,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="39.6">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -5867,7 +6010,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="39.6">
       <c r="A62" s="1" t="s">
         <v>193</v>
       </c>
@@ -5897,7 +6040,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="39.6">
       <c r="A63" s="1" t="s">
         <v>194</v>
       </c>
@@ -5927,7 +6070,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="39.6">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -5957,7 +6100,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="39.6">
       <c r="A65" s="1" t="s">
         <v>196</v>
       </c>
@@ -5987,7 +6130,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="26.4">
       <c r="A66" s="1" t="s">
         <v>197</v>
       </c>
@@ -6017,7 +6160,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="39.6">
       <c r="A67" s="1" t="s">
         <v>198</v>
       </c>
@@ -6047,7 +6190,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="39.6">
       <c r="A68" s="1" t="s">
         <v>199</v>
       </c>
@@ -6077,7 +6220,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="39.6">
       <c r="A69" s="1" t="s">
         <v>200</v>
       </c>
@@ -6107,7 +6250,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="39.6">
       <c r="A70" s="1" t="s">
         <v>201</v>
       </c>
@@ -6137,7 +6280,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="39.6">
       <c r="A71" s="1" t="s">
         <v>202</v>
       </c>
@@ -6167,7 +6310,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="39.6">
       <c r="A72" s="1" t="s">
         <v>203</v>
       </c>
@@ -6197,7 +6340,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="26.4">
       <c r="A74" s="1" t="s">
         <v>204</v>
       </c>
@@ -6227,7 +6370,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="39.6">
       <c r="A75" s="1" t="s">
         <v>208</v>
       </c>
@@ -6257,7 +6400,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="39.6">
       <c r="A76" s="1" t="s">
         <v>209</v>
       </c>
@@ -6287,7 +6430,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="26.4" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>213</v>
       </c>
@@ -6317,7 +6460,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="26.4">
       <c r="A79" s="1" t="s">
         <v>217</v>
       </c>
@@ -6347,7 +6490,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="26.4">
       <c r="A80" s="1" t="s">
         <v>218</v>
       </c>
@@ -6377,7 +6520,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="39.6">
       <c r="A81" s="1" t="s">
         <v>368</v>
       </c>
@@ -6407,7 +6550,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="39.6">
       <c r="A83" s="1" t="s">
         <v>224</v>
       </c>
@@ -6437,7 +6580,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="39.6">
       <c r="A84" s="1" t="s">
         <v>241</v>
       </c>
@@ -6467,7 +6610,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="39.6">
       <c r="A85" s="1" t="s">
         <v>242</v>
       </c>
@@ -6497,7 +6640,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="39.6">
       <c r="A86" s="1" t="s">
         <v>243</v>
       </c>
@@ -6527,7 +6670,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="39.6">
       <c r="A87" s="1" t="s">
         <v>244</v>
       </c>
@@ -6557,7 +6700,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="39.6">
       <c r="A88" s="1" t="s">
         <v>245</v>
       </c>
@@ -6587,7 +6730,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="39.6">
       <c r="A89" s="1" t="s">
         <v>246</v>
       </c>
@@ -6617,7 +6760,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="39.6">
       <c r="A90" s="1" t="s">
         <v>247</v>
       </c>
@@ -6647,7 +6790,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="39.6">
       <c r="A91" s="1" t="s">
         <v>248</v>
       </c>
@@ -6677,7 +6820,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="39.6">
       <c r="A92" s="1" t="s">
         <v>249</v>
       </c>
@@ -6707,7 +6850,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="39.6">
       <c r="A93" s="1" t="s">
         <v>250</v>
       </c>
@@ -6737,7 +6880,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="39.6">
       <c r="A94" s="1" t="s">
         <v>251</v>
       </c>
@@ -6767,7 +6910,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="26.4">
       <c r="A96" s="1" t="s">
         <v>252</v>
       </c>
@@ -6797,7 +6940,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="26.4">
       <c r="A97" s="1" t="s">
         <v>270</v>
       </c>
@@ -6827,7 +6970,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="26.4">
       <c r="A98" s="1" t="s">
         <v>271</v>
       </c>
@@ -6857,7 +7000,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="26.4">
       <c r="A99" s="1" t="s">
         <v>272</v>
       </c>
@@ -6887,7 +7030,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="26.4">
       <c r="A100" s="1" t="s">
         <v>273</v>
       </c>
@@ -6917,7 +7060,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="52.8">
       <c r="A101" s="1" t="s">
         <v>274</v>
       </c>
@@ -6947,7 +7090,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="26.4">
       <c r="A102" s="1" t="s">
         <v>275</v>
       </c>
@@ -6977,7 +7120,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="26.4">
       <c r="A103" s="1" t="s">
         <v>276</v>
       </c>
@@ -7007,7 +7150,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="26.4">
       <c r="A104" s="1" t="s">
         <v>277</v>
       </c>
@@ -7037,7 +7180,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="26.4">
       <c r="A105" s="1" t="s">
         <v>278</v>
       </c>
@@ -7067,7 +7210,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="26.4">
       <c r="A106" s="1" t="s">
         <v>279</v>
       </c>
@@ -7097,7 +7240,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="72.599999999999994" customHeight="1">
       <c r="A107" s="1" t="s">
         <v>280</v>
       </c>
@@ -7128,7 +7271,7 @@
       </c>
       <c r="K107" s="14"/>
     </row>
-    <row r="108" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="19.8" customHeight="1">
       <c r="B108" s="14"/>
       <c r="C108" s="14"/>
       <c r="D108" s="14"/>
@@ -7140,7 +7283,7 @@
       <c r="J108" s="14"/>
       <c r="K108" s="14"/>
     </row>
-    <row r="109" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="71.400000000000006" customHeight="1">
       <c r="A109" s="7" t="s">
         <v>283</v>
       </c>
@@ -7170,7 +7313,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="71.400000000000006" customHeight="1">
       <c r="A110" s="7" t="s">
         <v>290</v>
       </c>
@@ -7200,7 +7343,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="67.2" customHeight="1">
       <c r="A111" s="7" t="s">
         <v>291</v>
       </c>
@@ -7230,7 +7373,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="68.400000000000006" customHeight="1">
       <c r="A112" s="7" t="s">
         <v>292</v>
       </c>
@@ -7260,7 +7403,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="70.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="70.2" customHeight="1">
       <c r="A113" s="7" t="s">
         <v>293</v>
       </c>
@@ -7290,7 +7433,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="53.4" customHeight="1">
       <c r="A114" s="7" t="s">
         <v>294</v>
       </c>
@@ -7320,7 +7463,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="64.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="64.8" customHeight="1">
       <c r="A115" s="7" t="s">
         <v>295</v>
       </c>
@@ -7350,7 +7493,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="72" customHeight="1">
       <c r="A116" s="7" t="s">
         <v>296</v>
       </c>
@@ -7380,7 +7523,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="70.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="70.8" customHeight="1">
       <c r="A117" s="7" t="s">
         <v>297</v>
       </c>
@@ -7410,7 +7553,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="66" customHeight="1">
       <c r="A118" s="7" t="s">
         <v>298</v>
       </c>
@@ -7440,7 +7583,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="66" customHeight="1">
       <c r="A119" s="7" t="s">
         <v>299</v>
       </c>
@@ -7470,7 +7613,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="37.799999999999997" customHeight="1">
       <c r="A120" s="7" t="s">
         <v>300</v>
       </c>
@@ -7500,7 +7643,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="39.6">
       <c r="A122" s="1" t="s">
         <v>304</v>
       </c>
@@ -7530,7 +7673,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="39.6">
       <c r="A123" s="1" t="s">
         <v>320</v>
       </c>
@@ -7560,7 +7703,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="39.6">
       <c r="A124" s="1" t="s">
         <v>321</v>
       </c>
@@ -7590,7 +7733,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="39.6">
       <c r="A125" s="1" t="s">
         <v>322</v>
       </c>
@@ -7620,7 +7763,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="39.6">
       <c r="A126" s="1" t="s">
         <v>323</v>
       </c>
@@ -7650,7 +7793,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="52.8">
       <c r="A127" s="1" t="s">
         <v>324</v>
       </c>
@@ -7680,7 +7823,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="39.6">
       <c r="A128" s="1" t="s">
         <v>325</v>
       </c>
@@ -7710,7 +7853,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" ht="39.6">
       <c r="A129" s="1" t="s">
         <v>326</v>
       </c>
@@ -7740,7 +7883,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" ht="39.6">
       <c r="A130" s="1" t="s">
         <v>327</v>
       </c>
@@ -7770,7 +7913,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" ht="39.6">
       <c r="A131" s="1" t="s">
         <v>328</v>
       </c>
@@ -7800,7 +7943,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" ht="39.6">
       <c r="A132" s="1" t="s">
         <v>329</v>
       </c>
@@ -7830,7 +7973,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="39.6">
       <c r="A133" s="1" t="s">
         <v>330</v>
       </c>
@@ -7860,7 +8003,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" ht="54" customHeight="1">
       <c r="A135" s="1" t="s">
         <v>331</v>
       </c>
@@ -7890,7 +8033,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" ht="53.4" customHeight="1">
       <c r="A136" s="1" t="s">
         <v>344</v>
       </c>
@@ -7920,7 +8063,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" ht="51" customHeight="1">
       <c r="A137" s="1" t="s">
         <v>345</v>
       </c>
@@ -7950,7 +8093,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="52.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="52.2" customHeight="1">
       <c r="A138" s="1" t="s">
         <v>346</v>
       </c>
@@ -7980,7 +8123,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" ht="52.8" customHeight="1">
       <c r="A139" s="1" t="s">
         <v>347</v>
       </c>
@@ -8010,7 +8153,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" ht="58.8" customHeight="1">
       <c r="A140" s="1" t="s">
         <v>348</v>
       </c>
@@ -8040,7 +8183,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" ht="49.8" customHeight="1">
       <c r="A141" s="1" t="s">
         <v>349</v>
       </c>
@@ -8070,7 +8213,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" ht="49.2" customHeight="1">
       <c r="A142" s="1" t="s">
         <v>350</v>
       </c>
@@ -8100,7 +8243,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" ht="50.4" customHeight="1">
       <c r="A143" s="1" t="s">
         <v>351</v>
       </c>
@@ -8130,7 +8273,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" ht="50.4" customHeight="1">
       <c r="A144" s="1" t="s">
         <v>352</v>
       </c>
@@ -8160,7 +8303,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" ht="49.8" customHeight="1">
       <c r="A145" s="1" t="s">
         <v>353</v>
       </c>
@@ -8190,7 +8333,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" ht="49.2" customHeight="1">
       <c r="A146" s="1" t="s">
         <v>354</v>
       </c>
@@ -8220,7 +8363,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" ht="49.8" customHeight="1">
       <c r="A147" s="1" t="s">
         <v>355</v>
       </c>
@@ -8250,7 +8393,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" ht="53.4" customHeight="1">
       <c r="A148" s="1" t="s">
         <v>356</v>
       </c>
@@ -8280,7 +8423,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" ht="48.6" customHeight="1">
       <c r="A149" s="1" t="s">
         <v>366</v>
       </c>
@@ -8310,7 +8453,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="26.4">
       <c r="A151" s="1" t="s">
         <v>367</v>
       </c>
@@ -8340,7 +8483,7 @@
         <v>45425</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="92.4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" ht="92.4">
       <c r="A153" s="1" t="s">
         <v>378</v>
       </c>
@@ -8370,7 +8513,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="92.4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" ht="92.4">
       <c r="A154" s="1" t="s">
         <v>386</v>
       </c>
@@ -8400,7 +8543,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" ht="30" customHeight="1">
       <c r="A155" s="1" t="s">
         <v>416</v>
       </c>
@@ -8430,7 +8573,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="66" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" ht="66">
       <c r="A157" s="4" t="s">
         <v>387</v>
       </c>
@@ -8460,7 +8603,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="66" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" ht="66">
       <c r="A158" s="4" t="s">
         <v>397</v>
       </c>
@@ -8490,7 +8633,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="66" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" ht="66">
       <c r="A159" s="4" t="s">
         <v>398</v>
       </c>
@@ -8520,7 +8663,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="66" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" ht="66">
       <c r="A160" s="4" t="s">
         <v>399</v>
       </c>
@@ -8550,7 +8693,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="66" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="66">
       <c r="A161" s="4" t="s">
         <v>400</v>
       </c>
@@ -8580,7 +8723,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" ht="89.4" customHeight="1">
       <c r="A162" s="4" t="s">
         <v>401</v>
       </c>
@@ -8610,7 +8753,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="31.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" ht="81.599999999999994" customHeight="1">
       <c r="A163" s="4" t="s">
         <v>402</v>
       </c>
@@ -8640,7 +8783,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" ht="31.2" customHeight="1">
       <c r="A164" s="4" t="s">
         <v>403</v>
       </c>
@@ -8668,6 +8811,126 @@
       </c>
       <c r="J164" s="4">
         <v>45436</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="26.4">
+      <c r="A166" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E166" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="F166" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="G166" s="1"/>
+      <c r="H166" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J166" s="4">
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="26.4">
+      <c r="A167" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E167" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="G167" s="1"/>
+      <c r="H167" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J167" s="4">
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="26.4">
+      <c r="A168" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E168" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="F168" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="G168" s="1"/>
+      <c r="H168" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J168" s="4">
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="26.4">
+      <c r="A169" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E169" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="F169" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="G169" s="1"/>
+      <c r="H169" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J169" s="4">
+        <v>45439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>